<commit_message>
chore: ignore Office tempfiles (~$*.xlsx) en update sjablonenbestand voor live
</commit_message>
<xml_diff>
--- a/public/Sjablonen/25-26-Sjablonen-Return2Performance.xlsx
+++ b/public/Sjablonen/25-26-Sjablonen-Return2Performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\Sjablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B6FC3-22E3-4E3C-B99B-FB47FA96C8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98872905-3A4C-4665-9C26-88224E0AC496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-60" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sjablonen" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Naam</t>
   </si>
@@ -77,16 +77,43 @@
     <t>document</t>
   </si>
   <si>
-    <t>Portfolio Return2Performance</t>
-  </si>
-  <si>
-    <t>Portfolio Fit in the Hood</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
     <t>Behandelplan</t>
+  </si>
+  <si>
+    <t>Return2Performande</t>
+  </si>
+  <si>
+    <t>Fit in the Hood</t>
+  </si>
+  <si>
+    <t>Learn-2-Move</t>
+  </si>
+  <si>
+    <t>Choose-2-Move</t>
+  </si>
+  <si>
+    <t>Stay@Work</t>
+  </si>
+  <si>
+    <t>Explore Pain</t>
+  </si>
+  <si>
+    <t>Patient Journey</t>
+  </si>
+  <si>
+    <t>BVP1</t>
+  </si>
+  <si>
+    <t>BVP2</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Anamnese simulatie</t>
   </si>
 </sst>
 </file>
@@ -122,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -463,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -482,10 +510,10 @@
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="20" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,13 +545,37 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -551,16 +603,37 @@
       <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -570,6 +643,17 @@
       </c>
       <c r="J3" t="s">
         <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>